<commit_message>
Main Menu Screen Added for Read-me
</commit_message>
<xml_diff>
--- a/Price List.xlsx
+++ b/Price List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>Temperature Probe</t>
   </si>
@@ -103,6 +103,48 @@
   </si>
   <si>
     <t>' / 3</t>
+  </si>
+  <si>
+    <t>dry</t>
+  </si>
+  <si>
+    <t>burnt</t>
+  </si>
+  <si>
+    <t>Raw</t>
+  </si>
+  <si>
+    <t>Undercooked</t>
+  </si>
+  <si>
+    <t>Overcooked</t>
+  </si>
+  <si>
+    <t>Cooked</t>
+  </si>
+  <si>
+    <t>Slightly Cooked</t>
+  </si>
+  <si>
+    <t>Mean of Distribution</t>
+  </si>
+  <si>
+    <t>Varience</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Distribution</t>
+  </si>
+  <si>
+    <t>Distribution Probability</t>
+  </si>
+  <si>
+    <t>Std Deviation</t>
+  </si>
+  <si>
+    <t>Improvement</t>
   </si>
 </sst>
 </file>
@@ -149,12 +191,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -162,6 +205,151 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.40400503062117227"/>
+                  <c:y val="0.12776027996500439"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$49:$F$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>85000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>250000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="89553920"/>
+        <c:axId val="81769216"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="89553920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="81769216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="81769216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="89553920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.69812489063867034"/>
+          <c:y val="0.39313466025080207"/>
+          <c:w val="0.24280555555555555"/>
+          <c:h val="0.1674343832020998"/>
+        </c:manualLayout>
+      </c:layout>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -449,19 +637,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.85546875" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -474,7 +665,9 @@
       <c r="C1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
@@ -486,6 +679,9 @@
       </c>
       <c r="I1" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -496,22 +692,30 @@
         <v>3</v>
       </c>
       <c r="C2" s="2">
-        <f>ROUND($A$17*B2,0)</f>
+        <f t="shared" ref="C2:C9" si="0">ROUND($A$13*B2,0)</f>
         <v>9</v>
       </c>
+      <c r="D2" s="5">
+        <f t="shared" ref="D2:D8" si="1">0.025*C2</f>
+        <v>0.22500000000000001</v>
+      </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>1.4</v>
       </c>
       <c r="H2" s="2">
-        <f>ROUND(G2*$J$10*$J$12,0)</f>
-        <v>20</v>
+        <f>ROUND(G3*$J$10*$J$12,0)</f>
+        <v>12</v>
       </c>
       <c r="I2" s="2">
         <f>ROUND(G2*$J$10*$J$14,0)</f>
-        <v>44</v>
+        <v>31</v>
+      </c>
+      <c r="J2" s="5">
+        <f>0.025*(I2/$I$5)</f>
+        <v>4.3055555555555562E-2</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -522,53 +726,69 @@
         <v>1</v>
       </c>
       <c r="C3" s="2">
-        <f t="shared" ref="C3:C13" si="0">ROUND($A$17*B3,0)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
+      <c r="D3" s="5">
+        <f t="shared" si="1"/>
+        <v>7.5000000000000011E-2</v>
+      </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G3">
-        <v>1.75</v>
+        <v>1.2</v>
       </c>
       <c r="H3" s="2">
-        <f t="shared" ref="H3:H6" si="1">ROUND(G3*$J$10*$J$12,0)</f>
-        <v>18</v>
+        <f>ROUND(G2*$J$10*$J$12,0)</f>
+        <v>14</v>
       </c>
       <c r="I3" s="2">
-        <f t="shared" ref="I3:I6" si="2">ROUND(G3*$J$10*$J$14,0)</f>
-        <v>39</v>
+        <f>ROUND(G3*$J$10*$J$14,0)</f>
+        <v>26</v>
+      </c>
+      <c r="J3" s="5">
+        <f>0.025*(I3/$I$5)</f>
+        <v>3.6111111111111115E-2</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>15</v>
+      </c>
+      <c r="D4" s="5">
+        <f t="shared" si="1"/>
+        <v>0.375</v>
       </c>
       <c r="F4" t="s">
         <v>18</v>
       </c>
       <c r="G4">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="H4" s="2">
-        <f t="shared" si="1"/>
-        <v>13</v>
+        <f t="shared" ref="H4:H6" si="2">ROUND(G4*$J$10*$J$12,0)</f>
+        <v>10</v>
       </c>
       <c r="I4" s="2">
-        <f t="shared" si="2"/>
-        <v>28</v>
+        <f>ROUND(G4*$J$10*$J$14,0)</f>
+        <v>22</v>
+      </c>
+      <c r="J4" s="5">
+        <f>0.025*(I4/$I$5)</f>
+        <v>3.0555555555555558E-2</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -577,105 +797,126 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
+      <c r="D5" s="5">
+        <f t="shared" si="1"/>
+        <v>0.15000000000000002</v>
+      </c>
       <c r="F5" t="s">
         <v>17</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="H5" s="2">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="I5" s="2">
-        <f t="shared" si="2"/>
-        <v>22</v>
+        <f>ROUND(G5*$J$10*$J$14,0)</f>
+        <v>18</v>
+      </c>
+      <c r="J5" s="5">
+        <f>0.025*(I5/$I$5)</f>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>3</v>
+      </c>
+      <c r="D6" s="5">
+        <f t="shared" si="1"/>
+        <v>7.5000000000000011E-2</v>
       </c>
       <c r="F6" t="s">
         <v>16</v>
       </c>
       <c r="G6">
-        <v>0.85</v>
+        <v>0.6</v>
       </c>
       <c r="H6" s="2">
-        <f t="shared" si="1"/>
-        <v>9</v>
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
       <c r="I6" s="2">
-        <f t="shared" si="2"/>
-        <v>19</v>
+        <f>ROUND(G6*$J$10*$J$14,0)</f>
+        <v>13</v>
+      </c>
+      <c r="J6" s="5">
+        <f>0.025*(I6/$I$5)</f>
+        <v>1.8055555555555557E-2</v>
       </c>
     </row>
     <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
       <c r="C7" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D7" s="5">
+        <f t="shared" si="1"/>
+        <v>0.15000000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C8" s="2">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>3</v>
+      </c>
+      <c r="D8" s="5">
+        <f t="shared" si="1"/>
+        <v>7.5000000000000011E-2</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="C9" s="2">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="D9" s="5">
+        <f>0.025*C9</f>
+        <v>0.05</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
       <c r="J10" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
+      <c r="B11" t="s">
+        <v>27</v>
       </c>
       <c r="C11" s="2">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f>SUM(C2:C9)</f>
+        <v>47</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>22</v>
@@ -683,29 +924,23 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
+        <v>25</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="C12" s="2">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>C11/(COUNT(C2:C9)-3)</f>
+        <v>9.4</v>
       </c>
       <c r="J12">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13">
-        <v>0.5</v>
-      </c>
-      <c r="C13" s="2">
-        <f t="shared" si="0"/>
-        <v>2</v>
+      <c r="A13" s="2">
+        <f>3</f>
+        <v>3</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>23</v>
@@ -716,47 +951,156 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
-      <c r="B15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="2">
-        <f>SUM(C3:C13)</f>
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="2">
-        <f>C15/(COUNT(C2:C13)-3)</f>
-        <v>6.333333333333333</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="2">
-        <f>3</f>
-        <v>3</v>
-      </c>
-    </row>
     <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21">
+        <v>0.5</v>
+      </c>
+      <c r="C21" s="2">
+        <f>ROUND($A$13*B21,0)</f>
+        <v>2</v>
+      </c>
       <c r="F21" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" s="2">
+        <f>ROUND($A$13*B22,0)</f>
+        <v>6</v>
+      </c>
       <c r="F22" s="3">
-        <f>ROUND(I4+C16,0)</f>
+        <f>ROUND(I4+C12,0)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23">
+        <v>3.5</v>
+      </c>
+      <c r="C23" s="2">
+        <f>ROUND($A$13*B23,0)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="6:7">
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="6:11">
+      <c r="F49">
+        <v>5000</v>
+      </c>
+      <c r="G49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50" spans="6:11">
+      <c r="F50">
+        <v>10000</v>
+      </c>
+      <c r="G50" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="6:11">
+      <c r="F51">
+        <v>20000</v>
+      </c>
+      <c r="G51" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="52" spans="6:11">
+      <c r="F52">
+        <v>85000</v>
+      </c>
+      <c r="G52" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="53" spans="6:11">
+      <c r="F53">
+        <v>150000</v>
+      </c>
+      <c r="G53" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="54" spans="6:11">
+      <c r="F54">
+        <v>250000</v>
+      </c>
+      <c r="G54" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="56" spans="6:11">
+      <c r="G56" t="s">
+        <v>38</v>
+      </c>
+      <c r="H56" t="s">
+        <v>41</v>
+      </c>
+      <c r="I56" t="s">
+        <v>37</v>
+      </c>
+      <c r="J56" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="57" spans="6:11">
+      <c r="G57">
+        <v>100</v>
+      </c>
+      <c r="H57">
+        <f>SQRT(I57)</f>
+        <v>31.622776601683793</v>
+      </c>
+      <c r="I57">
+        <v>1000</v>
+      </c>
+      <c r="J57">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="59" spans="6:11">
+      <c r="J59" t="s">
+        <v>39</v>
+      </c>
+      <c r="K59">
+        <f>EXP(-((G57-J57)^2)/(2*I57))</f>
+        <v>0.14631404122463545</v>
+      </c>
+    </row>
+    <row r="61" spans="6:11">
+      <c r="J61" t="s">
+        <v>40</v>
+      </c>
+      <c r="K61">
+        <f>(1/SQRT(I57)*SQRT(2*PI()))*EXP(-((G57-J57)^2)/(2*I57))</f>
+        <v>1.1597808672172976E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>